<commit_message>
T1 Part 2 fixed b and m values
</commit_message>
<xml_diff>
--- a/T1/test.xlsx
+++ b/T1/test.xlsx
@@ -447,11 +447,11 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-0.0013037037042686027 + 0.03819400354120578 x**1 -
-0.4825396826849832 x**2 + 3.434941799789729 x**3 -
-15.09024444746217 x**4 + 42.07479630303774 x**5 - 73.58879630567384 x**6 +
-76.52075044869544 x**7 - 41.45211587650403 x**8 + 6.246317460972939 x**9 +
-6.000000000000381 x**10</t>
+          <t>-0.0013037037032453652 + 0.038194003516085574 x**1 -
+0.48253968242128487 x**2 + 3.434941798243592 x**3 -
+15.09024444191331 x**4 + 42.074796290477096 x**5 - 73.5887962878591 x**6 +
+76.52075043351839 x**7 - 41.45211586946449 x**8 + 6.246317459586915 x**9 +
+6.000000000008939 x**10</t>
         </is>
       </c>
     </row>

</xml_diff>